<commit_message>
fix the grammar of dataset section, and minor mistakes pointed by reviewer 1
</commit_message>
<xml_diff>
--- a/data/experiments/accession_metion_results.xlsx
+++ b/data/experiments/accession_metion_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26970" windowHeight="12510" activeTab="1"/>
+    <workbookView windowWidth="20175" windowHeight="12045" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="edge_for_each_mention" sheetId="1" r:id="rId1"/>
@@ -1381,19 +1381,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="17.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="14.7714285714286" customWidth="1"/>
     <col min="3" max="3" width="6.42857142857143" customWidth="1"/>
     <col min="4" max="4" width="12.8571428571429" customWidth="1"/>
     <col min="7" max="7" width="16.2857142857143"/>
+    <col min="8" max="8" width="12.8571428571429"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1497,7 +1498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1513,6 +1514,10 @@
       <c r="G8" s="3">
         <v>0.344109286964908</v>
       </c>
+      <c r="H8">
+        <f>G8^2*(800-1)/(800-1-1)</f>
+        <v>0.118559586339627</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
@@ -1528,7 +1533,7 @@
         <v>0.332817699740843</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1544,6 +1549,10 @@
       <c r="G10" s="3">
         <v>0.344109386582669</v>
       </c>
+      <c r="H10">
+        <f>D14^2*(800-1)/(800-1-3)</f>
+        <v>0.11669828897422</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
@@ -1671,36 +1680,36 @@
         <v>0.338306039976447</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24">
-        <v>20</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
         <v>0.05</v>
       </c>
-      <c r="D24">
+      <c r="D20">
         <v>0.341</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26">
+    <row r="21" spans="1:4">
+      <c r="A21">
         <v>100</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
         <v>0.05</v>
       </c>
-      <c r="D26">
+      <c r="D21">
         <v>0.343282489781861</v>
       </c>
     </row>
-    <row r="27" ht="15.75" spans="4:4">
-      <c r="D27" s="2"/>
+    <row r="22" ht="15.75" spans="4:4">
+      <c r="D22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>